<commit_message>
AI codes for transformations (S.P.O.)
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -529,39 +529,31 @@
           <t>Client Staff Visits</t>
         </is>
       </c>
-      <c r="C1" s="10" t="n"/>
-      <c r="D1" s="10" t="n"/>
-      <c r="E1" s="11" t="n"/>
       <c r="F1" s="12" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G1" s="12" t="n"/>
       <c r="H1" s="12" t="inlineStr">
         <is>
           <t>Series (Perf)</t>
         </is>
       </c>
-      <c r="I1" s="12" t="n"/>
       <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Products</t>
         </is>
       </c>
-      <c r="K1" s="12" t="n"/>
       <c r="L1" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="M1" s="12" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
           <t>Avg. Spend Per Client</t>
         </is>
       </c>
-      <c r="O1" s="12" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="2" t="n"/>
@@ -639,17 +631,17 @@
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>Maggie  Farrell</t>
+          <t>Chrissy Cummings</t>
         </is>
       </c>
       <c r="B3" s="10" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3" s="11" t="inlineStr">
         <is>
@@ -690,17 +682,17 @@
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>Makayla Baca</t>
+          <t>Danielle Mai</t>
         </is>
       </c>
       <c r="B4" s="10" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>7</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="11" t="inlineStr">
         <is>
@@ -741,17 +733,17 @@
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Justyne Martinez </t>
+          <t>Jasmine Saiz</t>
         </is>
       </c>
       <c r="B5" s="10" t="n">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D5" s="10" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="11" t="inlineStr">
         <is>
@@ -792,17 +784,17 @@
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Vy Torino</t>
+          <t>Karen Trevizo</t>
         </is>
       </c>
       <c r="B6" s="10" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Combines Whole #'s For Everyone Properly
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,17 +631,17 @@
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>Chrissy Cummings</t>
+          <t>Maggie  Farrell</t>
         </is>
       </c>
       <c r="B3" s="10" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" s="11" t="inlineStr">
         <is>
@@ -682,17 +682,17 @@
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>Danielle Mai</t>
+          <t>Makayla Baca</t>
         </is>
       </c>
       <c r="B4" s="10" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>7</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="11" t="inlineStr">
         <is>
@@ -733,17 +733,17 @@
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>Jasmine Saiz</t>
+          <t xml:space="preserve">Justyne Martinez </t>
         </is>
       </c>
       <c r="B5" s="10" t="n">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C5" s="10" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D5" s="10" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E5" s="11" t="inlineStr">
         <is>
@@ -784,17 +784,17 @@
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Karen Trevizo</t>
+          <t>Vy Torino</t>
         </is>
       </c>
       <c r="B6" s="10" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
@@ -1442,6 +1442,198 @@
       </c>
       <c r="O18" s="12" t="n">
         <v>10.78</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Aminah Avalos</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>34</v>
+      </c>
+      <c r="C20" t="n">
+        <v>14</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Chrissy Cummings</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>29</v>
+      </c>
+      <c r="C21" t="n">
+        <v>24</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Danielle Mai</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" t="n">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Izzy Kruis</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>44</v>
+      </c>
+      <c r="C23" t="n">
+        <v>24</v>
+      </c>
+      <c r="D23" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Jasmine Saiz</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>56</v>
+      </c>
+      <c r="C24" t="n">
+        <v>27</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Justyne Martinez </t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>25</v>
+      </c>
+      <c r="C25" t="n">
+        <v>15</v>
+      </c>
+      <c r="D25" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Karen Trevizo</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>27</v>
+      </c>
+      <c r="C26" t="n">
+        <v>21</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Krisdee Martinez</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>39</v>
+      </c>
+      <c r="C27" t="n">
+        <v>19</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Maggie  Farrell</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>38</v>
+      </c>
+      <c r="C28" t="n">
+        <v>20</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Makayla Baca</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>24</v>
+      </c>
+      <c r="C29" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Matthew Young</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Vy Torino</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>17</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6</v>
+      </c>
+      <c r="D31" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempt for all  in one transformation
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,31 +529,39 @@
           <t>Client Staff Visits</t>
         </is>
       </c>
+      <c r="C1" s="10" t="n"/>
+      <c r="D1" s="10" t="n"/>
+      <c r="E1" s="11" t="n"/>
       <c r="F1" s="12" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
+      <c r="G1" s="12" t="n"/>
       <c r="H1" s="12" t="inlineStr">
         <is>
           <t>Series (Perf)</t>
         </is>
       </c>
+      <c r="I1" s="12" t="n"/>
       <c r="J1" s="12" t="inlineStr">
         <is>
           <t>Products</t>
         </is>
       </c>
+      <c r="K1" s="12" t="n"/>
       <c r="L1" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
+      <c r="M1" s="12" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
           <t>Avg. Spend Per Client</t>
         </is>
       </c>
+      <c r="O1" s="12" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="2" t="n"/>
@@ -1442,198 +1450,6 @@
       </c>
       <c r="O18" s="12" t="n">
         <v>10.78</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Aminah Avalos</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>34</v>
-      </c>
-      <c r="C20" t="n">
-        <v>14</v>
-      </c>
-      <c r="D20" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Chrissy Cummings</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>29</v>
-      </c>
-      <c r="C21" t="n">
-        <v>24</v>
-      </c>
-      <c r="D21" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Danielle Mai</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>9</v>
-      </c>
-      <c r="C22" t="n">
-        <v>7</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Izzy Kruis</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>44</v>
-      </c>
-      <c r="C23" t="n">
-        <v>24</v>
-      </c>
-      <c r="D23" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>56</v>
-      </c>
-      <c r="C24" t="n">
-        <v>27</v>
-      </c>
-      <c r="D24" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Justyne Martinez </t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>25</v>
-      </c>
-      <c r="C25" t="n">
-        <v>15</v>
-      </c>
-      <c r="D25" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Karen Trevizo</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>27</v>
-      </c>
-      <c r="C26" t="n">
-        <v>21</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Krisdee Martinez</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>39</v>
-      </c>
-      <c r="C27" t="n">
-        <v>19</v>
-      </c>
-      <c r="D27" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Maggie  Farrell</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>38</v>
-      </c>
-      <c r="C28" t="n">
-        <v>20</v>
-      </c>
-      <c r="D28" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Makayla Baca</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>24</v>
-      </c>
-      <c r="C29" t="n">
-        <v>7</v>
-      </c>
-      <c r="D29" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Matthew Young</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Vy Torino</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>17</v>
-      </c>
-      <c r="C31" t="n">
-        <v>6</v>
-      </c>
-      <c r="D31" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully merged and consolidated
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,6 +1439,202 @@
         <v>76.38</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Chrissy Cummings</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>29</v>
+      </c>
+      <c r="C20" t="n">
+        <v>24</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2094</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2256.15</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2094</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2256.15</v>
+      </c>
+      <c r="N20" t="n">
+        <v>77.27500000000001</v>
+      </c>
+      <c r="O20" t="n">
+        <v>83.23999999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Danielle Mai</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" t="n">
+        <v>7</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>571</v>
+      </c>
+      <c r="G21" t="n">
+        <v>614.88</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>30</v>
+      </c>
+      <c r="K21" t="n">
+        <v>32.31</v>
+      </c>
+      <c r="L21" t="n">
+        <v>601</v>
+      </c>
+      <c r="M21" t="n">
+        <v>647.1899999999999</v>
+      </c>
+      <c r="N21" t="n">
+        <v>41.94</v>
+      </c>
+      <c r="O21" t="n">
+        <v>45.165</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jasmine Saiz</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>56</v>
+      </c>
+      <c r="C22" t="n">
+        <v>27</v>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4.550000000000001</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4107</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4425.11</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>4107</v>
+      </c>
+      <c r="M22" t="n">
+        <v>4425.11</v>
+      </c>
+      <c r="N22" t="n">
+        <v>77.245</v>
+      </c>
+      <c r="O22" t="n">
+        <v>83.205</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Karen Trevizo</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>27</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4.699999999999999</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1956</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2106.72</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>14</v>
+      </c>
+      <c r="K23" t="n">
+        <v>15.08</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1970</v>
+      </c>
+      <c r="M23" t="n">
+        <v>2121.8</v>
+      </c>
+      <c r="N23" t="n">
+        <v>72.83</v>
+      </c>
+      <c r="O23" t="n">
+        <v>78.45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
So close almost complete
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,202 +1439,6 @@
         <v>76.38</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Chrissy Cummings</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>29</v>
-      </c>
-      <c r="C20" t="n">
-        <v>24</v>
-      </c>
-      <c r="D20" t="n">
-        <v>6</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2094</v>
-      </c>
-      <c r="G20" t="n">
-        <v>2256.15</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2094</v>
-      </c>
-      <c r="M20" t="n">
-        <v>2256.15</v>
-      </c>
-      <c r="N20" t="n">
-        <v>72.20689655172414</v>
-      </c>
-      <c r="O20" t="n">
-        <v>77.79827586206896</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Danielle Mai</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>9</v>
-      </c>
-      <c r="C21" t="n">
-        <v>7</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>571</v>
-      </c>
-      <c r="G21" t="n">
-        <v>614.88</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>30</v>
-      </c>
-      <c r="K21" t="n">
-        <v>32.31</v>
-      </c>
-      <c r="L21" t="n">
-        <v>601</v>
-      </c>
-      <c r="M21" t="n">
-        <v>647.1899999999999</v>
-      </c>
-      <c r="N21" t="n">
-        <v>66.77777777777777</v>
-      </c>
-      <c r="O21" t="n">
-        <v>71.91</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>56</v>
-      </c>
-      <c r="C22" t="n">
-        <v>27</v>
-      </c>
-      <c r="D22" t="n">
-        <v>10</v>
-      </c>
-      <c r="E22" t="n">
-        <v>4.550000000000001</v>
-      </c>
-      <c r="F22" t="n">
-        <v>4107</v>
-      </c>
-      <c r="G22" t="n">
-        <v>4425.11</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>4107</v>
-      </c>
-      <c r="M22" t="n">
-        <v>4425.11</v>
-      </c>
-      <c r="N22" t="n">
-        <v>73.33928571428571</v>
-      </c>
-      <c r="O22" t="n">
-        <v>79.01982142857142</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Karen Trevizo</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>27</v>
-      </c>
-      <c r="C23" t="n">
-        <v>21</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="n">
-        <v>4.699999999999999</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1956</v>
-      </c>
-      <c r="G23" t="n">
-        <v>2106.72</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>14</v>
-      </c>
-      <c r="K23" t="n">
-        <v>15.08</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1970</v>
-      </c>
-      <c r="M23" t="n">
-        <v>2121.8</v>
-      </c>
-      <c r="N23" t="n">
-        <v>72.96296296296296</v>
-      </c>
-      <c r="O23" t="n">
-        <v>78.5851851851852</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Trying to get entire code to work
</commit_message>
<xml_diff>
--- a/StaffPerformanceOverviewtest-06-23 test copy.xlsx
+++ b/StaffPerformanceOverviewtest-06-23 test copy.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1034,28 +1034,26 @@
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Karen Trevizo</t>
+          <t>Chrissy Cummings</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.5</v>
       </c>
       <c r="F11" t="n">
-        <v>1376</v>
+        <v>2094</v>
       </c>
       <c r="G11" t="n">
-        <v>1481.76</v>
+        <v>2256.15</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1064,49 +1062,47 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>15.08</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1390</v>
+        <v>2094</v>
       </c>
       <c r="M11" t="n">
-        <v>1496.84</v>
+        <v>2256.15</v>
       </c>
       <c r="N11" t="n">
-        <v>73.16</v>
+        <v>72.20689655172414</v>
       </c>
       <c r="O11" t="n">
-        <v>78.78</v>
+        <v>77.79827586206896</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Karen Trevizo</t>
+          <t>Danielle Mai</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="G12" t="n">
-        <v>624.96</v>
+        <v>614.88</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1115,49 +1111,47 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>32.31</v>
       </c>
       <c r="L12" t="n">
-        <v>580</v>
+        <v>601</v>
       </c>
       <c r="M12" t="n">
-        <v>624.96</v>
+        <v>647.1899999999999</v>
       </c>
       <c r="N12" t="n">
-        <v>72.5</v>
+        <v>66.77777777777777</v>
       </c>
       <c r="O12" t="n">
-        <v>78.12</v>
+        <v>71.91</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Danielle Mai</t>
+          <t>Jasmine Saiz</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.550000000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>571</v>
+        <v>4107</v>
       </c>
       <c r="G13" t="n">
-        <v>614.88</v>
+        <v>4425.11</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1166,49 +1160,47 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>21.53</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>591</v>
+        <v>4107</v>
       </c>
       <c r="M13" t="n">
-        <v>636.41</v>
+        <v>4425.11</v>
       </c>
       <c r="N13" t="n">
-        <v>73.88</v>
+        <v>73.33928571428571</v>
       </c>
       <c r="O13" t="n">
-        <v>79.55</v>
+        <v>79.01982142857142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Danielle Mai</t>
+          <t>Karen Trevizo</t>
         </is>
       </c>
       <c r="B14" t="n">
+        <v>27</v>
+      </c>
+      <c r="C14" t="n">
+        <v>21</v>
+      </c>
+      <c r="D14" t="n">
         <v>1</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E14" t="n">
+        <v>4.699999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1956</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>2106.72</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1217,226 +1209,22 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K14" t="n">
-        <v>10.78</v>
+        <v>15.08</v>
       </c>
       <c r="L14" t="n">
-        <v>10</v>
+        <v>1970</v>
       </c>
       <c r="M14" t="n">
-        <v>10.78</v>
+        <v>2121.8</v>
       </c>
       <c r="N14" t="n">
-        <v>10</v>
+        <v>72.96296296296296</v>
       </c>
       <c r="O14" t="n">
-        <v>10.78</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>5</v>
-      </c>
-      <c r="C15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>410</v>
-      </c>
-      <c r="G15" t="n">
-        <v>441.51</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>410</v>
-      </c>
-      <c r="M15" t="n">
-        <v>441.51</v>
-      </c>
-      <c r="N15" t="n">
-        <v>82</v>
-      </c>
-      <c r="O15" t="n">
-        <v>88.3</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>51</v>
-      </c>
-      <c r="C16" t="n">
-        <v>22</v>
-      </c>
-      <c r="D16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>4.9</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>3697</v>
-      </c>
-      <c r="G16" t="n">
-        <v>3983.6</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>3697</v>
-      </c>
-      <c r="M16" t="n">
-        <v>3983.6</v>
-      </c>
-      <c r="N16" t="n">
-        <v>72.48999999999999</v>
-      </c>
-      <c r="O16" t="n">
-        <v>78.11</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Chrissy Cummings</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>251</v>
-      </c>
-      <c r="G17" t="n">
-        <v>270.29</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>251</v>
-      </c>
-      <c r="M17" t="n">
-        <v>270.29</v>
-      </c>
-      <c r="N17" t="n">
-        <v>83.67</v>
-      </c>
-      <c r="O17" t="n">
-        <v>90.09999999999999</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Chrissy Cummings</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>26</v>
-      </c>
-      <c r="C18" t="n">
-        <v>21</v>
-      </c>
-      <c r="D18" t="n">
-        <v>5</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>1843</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1985.86</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1843</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1985.86</v>
-      </c>
-      <c r="N18" t="n">
-        <v>70.88</v>
-      </c>
-      <c r="O18" t="n">
-        <v>76.38</v>
+        <v>78.5851851851852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>